<commit_message>
Re-ran statistical analyses with diurnal variation
</commit_message>
<xml_diff>
--- a/Model results Diurnal.xlsx
+++ b/Model results Diurnal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D15CBC-4246-3A41-8E5D-61ECEC7BE4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595D1286-96B2-584F-AE7F-CC341960F94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="23820" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,12 +530,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -748,7 +742,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -766,8 +760,6 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1126,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L5:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1420,7 +1412,7 @@
         <f t="shared" si="1"/>
         <v>0.89423076923076927</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="14">
         <f t="shared" si="2"/>
         <v>1.8942307692307694</v>
       </c>
@@ -1546,7 +1538,7 @@
         <f t="shared" si="1"/>
         <v>0.63855421686746983</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="14">
         <f t="shared" si="2"/>
         <v>1.0843373493975903</v>
       </c>
@@ -1614,7 +1606,7 @@
         <f t="shared" si="2"/>
         <v>0.96363636363636362</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="16">
         <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
@@ -1674,11 +1666,11 @@
         <f t="shared" si="1"/>
         <v>0.60240963855421692</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="14">
         <f t="shared" si="2"/>
         <v>1.2048192771084338</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="16">
         <f t="shared" si="3"/>
         <v>1.1084337349397591</v>
       </c>
@@ -1738,11 +1730,11 @@
         <f t="shared" si="1"/>
         <v>0.79268292682926833</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="14">
         <f t="shared" si="2"/>
         <v>1.7886178861788617</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="16">
         <f t="shared" si="3"/>
         <v>1.7073170731707317</v>
       </c>
@@ -1800,11 +1792,11 @@
         <f t="shared" si="1"/>
         <v>0.61478599221789887</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="14">
         <f t="shared" si="2"/>
         <v>1.4513618677042801</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="16">
         <f t="shared" si="3"/>
         <v>1.4980544747081712</v>
       </c>
@@ -1862,11 +1854,11 @@
         <f t="shared" si="1"/>
         <v>0.62650602409638556</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="14">
         <f t="shared" si="2"/>
         <v>3.1807228915662651</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="16">
         <f t="shared" si="3"/>
         <v>2.2730923694779115</v>
       </c>
@@ -2544,7 +2536,7 @@
       <c r="E23">
         <v>1.49</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
         <v>1</v>
       </c>
       <c r="G23" s="3">
@@ -2564,7 +2556,7 @@
         <f t="shared" si="1"/>
         <v>0.37718120805369132</v>
       </c>
-      <c r="L23" s="17">
+      <c r="L23" s="14">
         <f t="shared" si="2"/>
         <v>1.2818791946308725</v>
       </c>

</xml_diff>

<commit_message>
Fixed several issues associated with quantifying r in the DDE model for species with highly nonlinear trait responses
</commit_message>
<xml_diff>
--- a/Model results Diurnal.xlsx
+++ b/Model results Diurnal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595D1286-96B2-584F-AE7F-CC341960F94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A24D636-6D2B-E141-9F40-57C073245365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="500" windowWidth="23820" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +530,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -742,11 +748,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -760,7 +765,14 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1118,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L5:M23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,58 +1147,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1206,31 +1218,31 @@
       <c r="E2">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>0.113</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>0.109</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>6.3E-2</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <f>F2/$E2</f>
         <v>0.84328358208955223</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <f>G2/$E2</f>
         <v>0.58955223880597007</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <f>H2/$E2</f>
         <v>0.81343283582089543</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="15">
         <f>I2/$E2</f>
         <v>0.47014925373134325</v>
       </c>
@@ -1242,7 +1254,7 @@
         <f>M2-L2</f>
         <v>-0.34328358208955218</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="9">
         <f>(K2-J2)/J2</f>
         <v>-0.30088495575221247</v>
       </c>
@@ -1250,7 +1262,7 @@
         <f>(M2-L2)/L2</f>
         <v>-0.42201834862385318</v>
       </c>
-      <c r="R2" s="7"/>
+      <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1268,31 +1280,31 @@
       <c r="E3">
         <v>0.154</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0.12</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.151</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0.109</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>0.14299999999999999</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <f t="shared" ref="J3:J30" si="0">F3/$E3</f>
         <v>0.77922077922077915</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <f t="shared" ref="K3:K30" si="1">G3/$E3</f>
         <v>0.98051948051948046</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <f t="shared" ref="L3:L30" si="2">H3/$E3</f>
         <v>0.70779220779220775</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <f t="shared" ref="M3:M30" si="3">I3/$E3</f>
         <v>0.92857142857142849</v>
       </c>
@@ -1304,7 +1316,7 @@
         <f t="shared" ref="O3:O30" si="5">M3-L3</f>
         <v>0.22077922077922074</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="9">
         <f t="shared" ref="P3:P30" si="6">(K3-J3)/J3</f>
         <v>0.25833333333333336</v>
       </c>
@@ -1312,7 +1324,7 @@
         <f t="shared" ref="Q3:Q30" si="7">(M3-L3)/L3</f>
         <v>0.31192660550458712</v>
       </c>
-      <c r="R3" s="7"/>
+      <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1328,53 +1340,53 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>0.154</v>
-      </c>
-      <c r="F4" s="9">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F4" s="20">
         <v>0.12</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="21">
         <v>0.13700000000000001</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="22">
         <v>0.13300000000000001</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="21">
         <v>0.15</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <f t="shared" si="0"/>
-        <v>0.77922077922077915</v>
-      </c>
-      <c r="K4" s="14">
+        <v>1.3636363636363638</v>
+      </c>
+      <c r="K4" s="13">
         <f t="shared" si="1"/>
-        <v>0.88961038961038974</v>
-      </c>
-      <c r="L4" s="14">
+        <v>1.5568181818181821</v>
+      </c>
+      <c r="L4" s="13">
         <f t="shared" si="2"/>
-        <v>0.86363636363636365</v>
-      </c>
-      <c r="M4" s="16">
+        <v>1.5113636363636365</v>
+      </c>
+      <c r="M4" s="15">
         <f t="shared" si="3"/>
-        <v>0.97402597402597402</v>
+        <v>1.7045454545454546</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="4"/>
-        <v>0.11038961038961059</v>
+        <v>0.19318181818181834</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" si="5"/>
-        <v>0.11038961038961037</v>
-      </c>
-      <c r="P4" s="10">
+        <v>0.19318181818181812</v>
+      </c>
+      <c r="P4" s="9">
         <f t="shared" si="6"/>
-        <v>0.14166666666666694</v>
+        <v>0.14166666666666677</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" si="7"/>
         <v>0.12781954887218042</v>
       </c>
-      <c r="R4" s="7"/>
+      <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1390,53 +1402,53 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>0.104</v>
-      </c>
-      <c r="F5" s="8">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F5" s="23">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="21">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="21">
         <v>0.19700000000000001</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="21">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <f t="shared" si="0"/>
-        <v>0.75961538461538469</v>
-      </c>
-      <c r="K5" s="14">
+        <v>0.89772727272727282</v>
+      </c>
+      <c r="K5" s="13">
         <f t="shared" si="1"/>
-        <v>0.89423076923076927</v>
-      </c>
-      <c r="L5" s="14">
+        <v>1.0568181818181819</v>
+      </c>
+      <c r="L5" s="13">
         <f t="shared" si="2"/>
-        <v>1.8942307692307694</v>
-      </c>
-      <c r="M5" s="16">
+        <v>2.2386363636363638</v>
+      </c>
+      <c r="M5" s="15">
         <f t="shared" si="3"/>
-        <v>0.95192307692307698</v>
+        <v>1.1250000000000002</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="4"/>
-        <v>0.13461538461538458</v>
+        <v>0.15909090909090906</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
-        <v>-0.9423076923076924</v>
-      </c>
-      <c r="P5" s="10">
+        <v>-1.1136363636363635</v>
+      </c>
+      <c r="P5" s="9">
         <f t="shared" si="6"/>
         <v>0.17721518987341767</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="7"/>
-        <v>-0.49746192893401014</v>
-      </c>
-      <c r="R5" s="7"/>
+        <v>-0.49746192893401009</v>
+      </c>
+      <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1454,31 +1466,31 @@
       <c r="E6">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>5.5E-2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <f t="shared" si="0"/>
         <v>0.61818181818181817</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <f t="shared" si="1"/>
         <v>0.31515151515151513</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f t="shared" si="2"/>
         <v>0.61818181818181817</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="15">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
@@ -1490,7 +1502,7 @@
         <f t="shared" si="5"/>
         <v>-0.28484848484848485</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="9">
         <f t="shared" si="6"/>
         <v>-0.49019607843137258</v>
       </c>
@@ -1498,7 +1510,7 @@
         <f t="shared" si="7"/>
         <v>-0.46078431372549022</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1518,31 +1530,31 @@
       <c r="E7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>0.09</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <f t="shared" si="0"/>
         <v>0.59036144578313254</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <f t="shared" si="1"/>
         <v>0.63855421686746983</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f t="shared" si="2"/>
         <v>1.0843373493975903</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <f t="shared" si="3"/>
         <v>0.77108433734939752</v>
       </c>
@@ -1554,7 +1566,7 @@
         <f t="shared" si="5"/>
         <v>-0.31325301204819278</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="9">
         <f t="shared" si="6"/>
         <v>8.1632653061224372E-2</v>
       </c>
@@ -1562,7 +1574,7 @@
         <f t="shared" si="7"/>
         <v>-0.28888888888888892</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="R7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1582,31 +1594,31 @@
       <c r="E8">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>0.104</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.10299999999999999</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.159</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>0.22</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <f t="shared" si="0"/>
         <v>0.63030303030303025</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="13">
         <f t="shared" si="1"/>
         <v>0.62424242424242415</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f t="shared" si="2"/>
         <v>0.96363636363636362</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="15">
         <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
@@ -1618,7 +1630,7 @@
         <f t="shared" si="5"/>
         <v>0.36969696969696964</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <f t="shared" si="6"/>
         <v>-9.6153846153846784E-3</v>
       </c>
@@ -1626,7 +1638,7 @@
         <f t="shared" si="7"/>
         <v>0.38364779874213828</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1646,31 +1658,31 @@
       <c r="E9">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.05</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>0.05</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>0.1</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <f t="shared" si="0"/>
         <v>0.60240963855421692</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <f t="shared" si="1"/>
         <v>0.60240963855421692</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f t="shared" si="2"/>
         <v>1.2048192771084338</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="15">
         <f t="shared" si="3"/>
         <v>1.1084337349397591</v>
       </c>
@@ -1682,7 +1694,7 @@
         <f t="shared" si="5"/>
         <v>-9.6385542168674787E-2</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -1690,7 +1702,7 @@
         <f t="shared" si="7"/>
         <v>-8.0000000000000071E-2</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1710,31 +1722,31 @@
       <c r="E10">
         <v>0.246</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.19900000000000001</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>0.19500000000000001</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>0.44</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>0.42</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <f t="shared" si="0"/>
         <v>0.80894308943089432</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <f t="shared" si="1"/>
         <v>0.79268292682926833</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="13">
         <f t="shared" si="2"/>
         <v>1.7886178861788617</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="15">
         <f t="shared" si="3"/>
         <v>1.7073170731707317</v>
       </c>
@@ -1746,7 +1758,7 @@
         <f t="shared" si="5"/>
         <v>-8.1300813008130079E-2</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <f t="shared" si="6"/>
         <v>-2.0100502512562787E-2</v>
       </c>
@@ -1754,7 +1766,7 @@
         <f t="shared" si="7"/>
         <v>-4.5454545454545456E-2</v>
       </c>
-      <c r="R10" s="7"/>
+      <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1772,31 +1784,31 @@
       <c r="E11">
         <v>0.25700000000000001</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.185</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>0.158</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.373</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>0.38500000000000001</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <f t="shared" si="0"/>
         <v>0.71984435797665369</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <f t="shared" si="1"/>
         <v>0.61478599221789887</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="13">
         <f t="shared" si="2"/>
         <v>1.4513618677042801</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="15">
         <f t="shared" si="3"/>
         <v>1.4980544747081712</v>
       </c>
@@ -1808,7 +1820,7 @@
         <f t="shared" si="5"/>
         <v>4.6692607003891107E-2</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="9">
         <f t="shared" si="6"/>
         <v>-0.1459459459459459</v>
       </c>
@@ -1816,7 +1828,7 @@
         <f t="shared" si="7"/>
         <v>3.217158176943704E-2</v>
       </c>
-      <c r="R11" s="7"/>
+      <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1834,31 +1846,31 @@
       <c r="E12">
         <v>0.249</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>0.183</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>0.156</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>0.79200000000000004</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>0.56599999999999995</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <f t="shared" si="0"/>
         <v>0.73493975903614461</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="13">
         <f t="shared" si="1"/>
         <v>0.62650602409638556</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="13">
         <f t="shared" si="2"/>
         <v>3.1807228915662651</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="15">
         <f t="shared" si="3"/>
         <v>2.2730923694779115</v>
       </c>
@@ -1870,7 +1882,7 @@
         <f t="shared" si="5"/>
         <v>-0.9076305220883536</v>
       </c>
-      <c r="P12" s="10">
+      <c r="P12" s="9">
         <f t="shared" si="6"/>
         <v>-0.1475409836065574</v>
       </c>
@@ -1878,7 +1890,7 @@
         <f t="shared" si="7"/>
         <v>-0.28535353535353541</v>
       </c>
-      <c r="R12" s="7"/>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1896,7 +1908,7 @@
       <c r="E13" s="1">
         <v>0.1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="G13" s="1">
@@ -1905,22 +1917,22 @@
       <c r="H13" s="1">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <f t="shared" si="0"/>
         <v>0.61</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="13">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <f t="shared" si="2"/>
         <v>0.73999999999999988</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="15">
         <f t="shared" si="3"/>
         <v>0.78999999999999992</v>
       </c>
@@ -1932,7 +1944,7 @@
         <f t="shared" si="5"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13" s="9">
         <f t="shared" si="6"/>
         <v>-0.5901639344262295</v>
       </c>
@@ -1940,7 +1952,7 @@
         <f t="shared" si="7"/>
         <v>6.7567567567567641E-2</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1960,7 +1972,7 @@
       <c r="E14">
         <v>0.104</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="G14" s="1">
@@ -1969,22 +1981,22 @@
       <c r="H14" s="1">
         <v>7.8E-2</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <f t="shared" si="0"/>
         <v>0.56730769230769229</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="13">
         <f t="shared" si="1"/>
         <v>-0.14423076923076925</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="13">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="15">
         <f t="shared" si="3"/>
         <v>0.78846153846153855</v>
       </c>
@@ -1996,7 +2008,7 @@
         <f t="shared" si="5"/>
         <v>3.8461538461538547E-2</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="9">
         <f t="shared" si="6"/>
         <v>-1.2542372881355932</v>
       </c>
@@ -2004,7 +2016,7 @@
         <f t="shared" si="7"/>
         <v>5.1282051282051398E-2</v>
       </c>
-      <c r="R14" s="7" t="s">
+      <c r="R14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2024,7 +2036,7 @@
       <c r="E15">
         <v>0.48399999999999999</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>0.23400000000000001</v>
       </c>
       <c r="G15" s="1">
@@ -2036,19 +2048,19 @@
       <c r="I15">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <f t="shared" si="0"/>
         <v>0.48347107438016534</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="13">
         <f t="shared" si="1"/>
         <v>0.40495867768595045</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="13">
         <f t="shared" si="2"/>
         <v>0.27272727272727276</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <f t="shared" si="3"/>
         <v>0.18388429752066116</v>
       </c>
@@ -2060,7 +2072,7 @@
         <f t="shared" si="5"/>
         <v>-8.8842975206611607E-2</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="9">
         <f t="shared" si="6"/>
         <v>-0.1623931623931624</v>
       </c>
@@ -2068,7 +2080,7 @@
         <f t="shared" si="7"/>
         <v>-0.32575757575757586</v>
       </c>
-      <c r="R15" s="7" t="s">
+      <c r="R15" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2088,7 +2100,7 @@
       <c r="E16">
         <v>0.436</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>0.24</v>
       </c>
       <c r="G16" s="1">
@@ -2100,19 +2112,19 @@
       <c r="I16">
         <v>7.8E-2</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="8">
         <f t="shared" si="0"/>
         <v>0.55045871559633031</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="13">
         <f t="shared" si="1"/>
         <v>0.50688073394495414</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <f t="shared" si="2"/>
         <v>0.24770642201834861</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="15">
         <f t="shared" si="3"/>
         <v>0.17889908256880735</v>
       </c>
@@ -2124,7 +2136,7 @@
         <f t="shared" si="5"/>
         <v>-6.880733944954126E-2</v>
       </c>
-      <c r="P16" s="10">
+      <c r="P16" s="9">
         <f t="shared" si="6"/>
         <v>-7.9166666666666691E-2</v>
       </c>
@@ -2132,7 +2144,7 @@
         <f t="shared" si="7"/>
         <v>-0.27777777777777768</v>
       </c>
-      <c r="R16" s="7" t="s">
+      <c r="R16" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2152,31 +2164,31 @@
       <c r="E17">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="16">
         <v>0.12</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="17">
         <v>0.154</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="17">
         <v>0.155</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="18">
         <v>0.11600000000000001</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <f t="shared" si="0"/>
         <v>0.41958041958041958</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="13">
         <f t="shared" si="1"/>
         <v>0.53846153846153855</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="13">
         <f t="shared" si="2"/>
         <v>0.54195804195804198</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="15">
         <f t="shared" si="3"/>
         <v>0.40559440559440563</v>
       </c>
@@ -2188,7 +2200,7 @@
         <f t="shared" si="5"/>
         <v>-0.13636363636363635</v>
       </c>
-      <c r="P17" s="10">
+      <c r="P17" s="9">
         <f t="shared" si="6"/>
         <v>0.28333333333333355</v>
       </c>
@@ -2196,7 +2208,7 @@
         <f t="shared" si="7"/>
         <v>-0.25161290322580643</v>
       </c>
-      <c r="R17" s="7" t="s">
+      <c r="R17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2216,7 +2228,7 @@
       <c r="E18">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>0.14399999999999999</v>
       </c>
       <c r="G18" s="1">
@@ -2228,19 +2240,19 @@
       <c r="I18">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <f t="shared" si="0"/>
         <v>0.74226804123711332</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="13">
         <f t="shared" si="1"/>
         <v>0.89690721649484528</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="13">
         <f t="shared" si="2"/>
         <v>0.46391752577319584</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18" s="15">
         <f t="shared" si="3"/>
         <v>0.52577319587628857</v>
       </c>
@@ -2252,7 +2264,7 @@
         <f t="shared" si="5"/>
         <v>6.185567010309273E-2</v>
       </c>
-      <c r="P18" s="10">
+      <c r="P18" s="9">
         <f t="shared" si="6"/>
         <v>0.20833333333333337</v>
       </c>
@@ -2260,7 +2272,7 @@
         <f t="shared" si="7"/>
         <v>0.13333333333333322</v>
       </c>
-      <c r="R18" s="7" t="s">
+      <c r="R18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2280,7 +2292,7 @@
       <c r="E19">
         <v>0.443</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>0.34499999999999997</v>
       </c>
       <c r="G19" s="1">
@@ -2289,22 +2301,22 @@
       <c r="H19" s="1">
         <v>0.186</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <f t="shared" si="0"/>
         <v>0.77878103837471779</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="13">
         <f t="shared" si="1"/>
         <v>0.72009029345372466</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="13">
         <f t="shared" si="2"/>
         <v>0.41986455981941306</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="15">
         <f t="shared" si="3"/>
         <v>0.23024830699774265</v>
       </c>
@@ -2316,7 +2328,7 @@
         <f t="shared" si="5"/>
         <v>-0.18961625282167041</v>
       </c>
-      <c r="P19" s="10">
+      <c r="P19" s="9">
         <f t="shared" si="6"/>
         <v>-7.536231884057959E-2</v>
       </c>
@@ -2324,7 +2336,7 @@
         <f t="shared" si="7"/>
         <v>-0.45161290322580644</v>
       </c>
-      <c r="R19" s="7" t="s">
+      <c r="R19" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2344,7 +2356,7 @@
       <c r="E20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>0.247</v>
       </c>
       <c r="G20" s="1">
@@ -2356,19 +2368,19 @@
       <c r="I20" s="1">
         <v>0.19700000000000001</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <f t="shared" si="0"/>
         <v>0.80718954248366015</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <f t="shared" si="1"/>
         <v>0.88235294117647067</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="13">
         <f t="shared" si="2"/>
         <v>0.60130718954248363</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="15">
         <f t="shared" si="3"/>
         <v>0.64379084967320266</v>
       </c>
@@ -2380,7 +2392,7 @@
         <f t="shared" si="5"/>
         <v>4.2483660130719025E-2</v>
       </c>
-      <c r="P20" s="10">
+      <c r="P20" s="9">
         <f t="shared" si="6"/>
         <v>9.3117408906882665E-2</v>
       </c>
@@ -2388,7 +2400,7 @@
         <f t="shared" si="7"/>
         <v>7.0652173913043598E-2</v>
       </c>
-      <c r="R20" s="7" t="s">
+      <c r="R20" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2408,7 +2420,7 @@
       <c r="E21">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>0.11899999999999999</v>
       </c>
       <c r="G21" s="1">
@@ -2420,19 +2432,19 @@
       <c r="I21">
         <v>0.106</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <f t="shared" si="0"/>
         <v>0.59798994974874364</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="13">
         <f t="shared" si="1"/>
         <v>0.59296482412060292</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="13">
         <f t="shared" si="2"/>
         <v>0.52763819095477382</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21" s="15">
         <f t="shared" si="3"/>
         <v>0.53266331658291455</v>
       </c>
@@ -2444,7 +2456,7 @@
         <f t="shared" si="5"/>
         <v>5.0251256281407253E-3</v>
       </c>
-      <c r="P21" s="10">
+      <c r="P21" s="9">
         <f t="shared" si="6"/>
         <v>-8.4033613445378529E-3</v>
       </c>
@@ -2452,7 +2464,7 @@
         <f t="shared" si="7"/>
         <v>9.5238095238095663E-3</v>
       </c>
-      <c r="R21" s="7" t="s">
+      <c r="R21" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2472,7 +2484,7 @@
       <c r="E22">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>0.112</v>
       </c>
       <c r="G22" s="1">
@@ -2484,19 +2496,19 @@
       <c r="I22" s="1">
         <v>0.09</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="8">
         <f t="shared" si="0"/>
         <v>0.5490196078431373</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="13">
         <f t="shared" si="1"/>
         <v>0.37745098039215691</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="13">
         <f t="shared" si="2"/>
         <v>0.40686274509803927</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="15">
         <f t="shared" si="3"/>
         <v>0.44117647058823528</v>
       </c>
@@ -2508,7 +2520,7 @@
         <f t="shared" si="5"/>
         <v>3.4313725490196012E-2</v>
       </c>
-      <c r="P22" s="10">
+      <c r="P22" s="9">
         <f t="shared" si="6"/>
         <v>-0.3125</v>
       </c>
@@ -2516,7 +2528,7 @@
         <f t="shared" si="7"/>
         <v>8.4337349397590189E-2</v>
       </c>
-      <c r="R22" s="7" t="s">
+      <c r="R22" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2536,31 +2548,31 @@
       <c r="E23">
         <v>1.49</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="19">
         <v>1</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="17">
         <v>0.56200000000000006</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="17">
         <v>1.91</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="18">
         <v>0.255</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="8">
         <f t="shared" si="0"/>
         <v>0.67114093959731547</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="13">
         <f t="shared" si="1"/>
         <v>0.37718120805369132</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="13">
         <f t="shared" si="2"/>
         <v>1.2818791946308725</v>
       </c>
-      <c r="M23" s="16">
+      <c r="M23" s="15">
         <f t="shared" si="3"/>
         <v>0.17114093959731544</v>
       </c>
@@ -2572,7 +2584,7 @@
         <f t="shared" si="5"/>
         <v>-1.1107382550335572</v>
       </c>
-      <c r="P23" s="10">
+      <c r="P23" s="9">
         <f t="shared" si="6"/>
         <v>-0.43799999999999994</v>
       </c>
@@ -2580,7 +2592,7 @@
         <f t="shared" si="7"/>
         <v>-0.86649214659685869</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="R23" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2600,7 +2612,7 @@
       <c r="E24">
         <v>3.42</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <v>1.67</v>
       </c>
       <c r="G24" s="1">
@@ -2612,19 +2624,19 @@
       <c r="I24">
         <v>2.7E-2</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <f t="shared" si="0"/>
         <v>0.48830409356725146</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K24" s="13">
         <f t="shared" si="1"/>
         <v>0.26432748538011697</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="13">
         <f t="shared" si="2"/>
         <v>0.25321637426900584</v>
       </c>
-      <c r="M24" s="16">
+      <c r="M24" s="15">
         <f t="shared" si="3"/>
         <v>7.8947368421052634E-3</v>
       </c>
@@ -2636,7 +2648,7 @@
         <f t="shared" si="5"/>
         <v>-0.24532163742690058</v>
       </c>
-      <c r="P24" s="10">
+      <c r="P24" s="9">
         <f t="shared" si="6"/>
         <v>-0.45868263473053889</v>
       </c>
@@ -2644,7 +2656,7 @@
         <f t="shared" si="7"/>
         <v>-0.96882217090069289</v>
       </c>
-      <c r="R24" s="7" t="s">
+      <c r="R24" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2664,7 +2676,7 @@
       <c r="E25">
         <v>0.33200000000000002</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>0.222</v>
       </c>
       <c r="G25" s="1">
@@ -2676,19 +2688,19 @@
       <c r="I25">
         <v>0.189</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <f t="shared" si="0"/>
         <v>0.66867469879518071</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="13">
         <f t="shared" si="1"/>
         <v>0.62048192771084332</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="13">
         <f t="shared" si="2"/>
         <v>0.51204819277108438</v>
       </c>
-      <c r="M25" s="16">
+      <c r="M25" s="15">
         <f t="shared" si="3"/>
         <v>0.56927710843373491</v>
       </c>
@@ -2700,7 +2712,7 @@
         <f t="shared" si="5"/>
         <v>5.7228915662650537E-2</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P25" s="9">
         <f t="shared" si="6"/>
         <v>-7.2072072072072141E-2</v>
       </c>
@@ -2708,7 +2720,7 @@
         <f t="shared" si="7"/>
         <v>0.11176470588235281</v>
       </c>
-      <c r="R25" s="7" t="s">
+      <c r="R25" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2728,7 +2740,7 @@
       <c r="E26">
         <v>0.39700000000000002</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="9">
         <v>0.22</v>
       </c>
       <c r="G26" s="1">
@@ -2740,19 +2752,19 @@
       <c r="I26">
         <v>0.20799999999999999</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <f t="shared" si="0"/>
         <v>0.55415617128463479</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="13">
         <f t="shared" si="1"/>
         <v>0.51889168765743066</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="13">
         <f t="shared" si="2"/>
         <v>0.55415617128463479</v>
       </c>
-      <c r="M26" s="16">
+      <c r="M26" s="15">
         <f t="shared" si="3"/>
         <v>0.52392947103274556</v>
       </c>
@@ -2764,7 +2776,7 @@
         <f t="shared" si="5"/>
         <v>-3.0226700251889227E-2</v>
       </c>
-      <c r="P26" s="10">
+      <c r="P26" s="9">
         <f t="shared" si="6"/>
         <v>-6.3636363636363824E-2</v>
       </c>
@@ -2772,7 +2784,7 @@
         <f t="shared" si="7"/>
         <v>-5.4545454545454647E-2</v>
       </c>
-      <c r="R26" s="7" t="s">
+      <c r="R26" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2792,7 +2804,7 @@
       <c r="E27">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="9">
         <v>0.23899999999999999</v>
       </c>
       <c r="G27" s="1">
@@ -2804,19 +2816,19 @@
       <c r="I27">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <f t="shared" si="0"/>
         <v>0.51508620689655171</v>
       </c>
-      <c r="K27" s="14">
+      <c r="K27" s="13">
         <f t="shared" si="1"/>
         <v>9.4827586206896547E-2</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="13">
         <f t="shared" si="2"/>
         <v>0.49137931034482757</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="15">
         <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
@@ -2828,7 +2840,7 @@
         <f t="shared" si="5"/>
         <v>-0.36637931034482757</v>
       </c>
-      <c r="P27" s="10">
+      <c r="P27" s="9">
         <f t="shared" si="6"/>
         <v>-0.81589958158995812</v>
       </c>
@@ -2836,7 +2848,7 @@
         <f t="shared" si="7"/>
         <v>-0.74561403508771928</v>
       </c>
-      <c r="R27" s="7" t="s">
+      <c r="R27" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2856,7 +2868,7 @@
       <c r="E28">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="9">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G28" s="1">
@@ -2868,19 +2880,19 @@
       <c r="I28">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <f t="shared" si="0"/>
         <v>0.30215827338129497</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="13">
         <f>G28/$E28</f>
         <v>-1.8129496402877696</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L28" s="13">
         <f t="shared" si="2"/>
         <v>0.15827338129496402</v>
       </c>
-      <c r="M28" s="16">
+      <c r="M28" s="15">
         <f t="shared" si="3"/>
         <v>-5.0359712230215826E-2</v>
       </c>
@@ -2892,7 +2904,7 @@
         <f>M28-L28</f>
         <v>-0.20863309352517984</v>
       </c>
-      <c r="P28" s="10">
+      <c r="P28" s="9">
         <f>(K28-J28)/ABS(J28)</f>
         <v>-6.9999999999999991</v>
       </c>
@@ -2900,7 +2912,7 @@
         <f t="shared" si="7"/>
         <v>-1.3181818181818181</v>
       </c>
-      <c r="R28" s="7" t="s">
+      <c r="R28" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2920,7 +2932,7 @@
       <c r="E29">
         <v>0.29899999999999999</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="9">
         <v>0.127</v>
       </c>
       <c r="G29" s="1">
@@ -2932,19 +2944,19 @@
       <c r="I29">
         <v>6.3E-2</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <f t="shared" si="0"/>
         <v>0.42474916387959871</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="13">
         <f t="shared" si="1"/>
         <v>-0.85953177257525093</v>
       </c>
-      <c r="L29" s="14">
+      <c r="L29" s="13">
         <f t="shared" si="2"/>
         <v>0.57525083612040129</v>
       </c>
-      <c r="M29" s="16">
+      <c r="M29" s="15">
         <f t="shared" si="3"/>
         <v>0.21070234113712374</v>
       </c>
@@ -2956,7 +2968,7 @@
         <f t="shared" si="5"/>
         <v>-0.36454849498327757</v>
       </c>
-      <c r="P29" s="10">
+      <c r="P29" s="9">
         <f t="shared" si="6"/>
         <v>-3.023622047244094</v>
       </c>
@@ -2964,7 +2976,7 @@
         <f t="shared" si="7"/>
         <v>-0.63372093023255816</v>
       </c>
-      <c r="R29" s="7" t="s">
+      <c r="R29" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2984,7 +2996,7 @@
       <c r="E30">
         <v>0.35699999999999998</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="9">
         <v>0.19</v>
       </c>
       <c r="G30" s="1">
@@ -2996,19 +3008,19 @@
       <c r="I30" s="1">
         <v>0.11</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <f t="shared" si="0"/>
         <v>0.53221288515406162</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="13">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L30" s="14">
+      <c r="L30" s="13">
         <f t="shared" si="2"/>
         <v>0.60784313725490202</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="15">
         <f t="shared" si="3"/>
         <v>0.3081232492997199</v>
       </c>
@@ -3020,7 +3032,7 @@
         <f t="shared" si="5"/>
         <v>-0.29971988795518212</v>
       </c>
-      <c r="P30" s="10">
+      <c r="P30" s="9">
         <f t="shared" si="6"/>
         <v>-0.37368421052631584</v>
       </c>
@@ -3028,7 +3040,7 @@
         <f t="shared" si="7"/>
         <v>-0.49308755760368667</v>
       </c>
-      <c r="R30" s="7" t="s">
+      <c r="R30" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>